<commit_message>
States not mentioned → ?
</commit_message>
<xml_diff>
--- a/Project5186_A. B. Smith(2001).xlsx
+++ b/Project5186_A. B. Smith(2001).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/remi/Desktop/Finished &amp; Uploaded copy 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjg18\GitHub\neotrans\matrices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EA2F3A-8BB7-3947-A241-9F9CCB8DAA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE95770D-E1F9-4184-891B-1A669A1EA804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{28D8B22D-54DF-6344-835A-EC7ACC6747D3}"/>
+    <workbookView xWindow="16245" yWindow="6825" windowWidth="15870" windowHeight="18585" xr2:uid="{28D8B22D-54DF-6344-835A-EC7ACC6747D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Project5186" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="51">
   <si>
     <t>Charlabels</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>T?;0=0;1=1;2=?</t>
+  </si>
+  <si>
+    <t>T?;0=0;1=1;2=2;3=?</t>
+  </si>
+  <si>
+    <t>N;0=0;1=1;2=?</t>
   </si>
 </sst>
 </file>
@@ -627,17 +636,17 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.1640625" customWidth="1"/>
+    <col min="1" max="1" width="83.125" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -659,7 +668,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -670,7 +679,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -681,7 +690,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -692,7 +701,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -703,7 +712,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -714,18 +723,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -736,7 +745,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -747,7 +756,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -758,18 +767,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -780,7 +789,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -791,7 +800,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -802,7 +811,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -813,7 +822,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -824,7 +833,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -835,18 +844,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -857,18 +866,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -879,18 +888,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -901,7 +910,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -912,18 +921,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -934,7 +943,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -945,7 +954,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -956,7 +965,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -967,18 +976,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -989,7 +998,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1000,18 +1009,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1022,18 +1031,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1044,18 +1053,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1066,7 +1075,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1077,18 +1086,18 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>

</xml_diff>